<commit_message>
Add SQL script for calculating mutual friends count with two solutions
</commit_message>
<xml_diff>
--- a/Mutual_Friends_Count/Problem_Statement.xlsx
+++ b/Mutual_Friends_Count/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q15/Video_Q15_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Mutual_Friends_Count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA64922-D6A3-3943-8290-8BAE82156E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAD7F0E-54F1-4926-870A-E494DDE8411A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{E2B8983A-410F-1E4E-B9F8-70A3BE661D0C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{E2B8983A-410F-1E4E-B9F8-70A3BE661D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -66,9 +64,6 @@
   </si>
   <si>
     <t>OUTPUT</t>
-  </si>
-  <si>
-    <t>Video #15 - Mutual Friends count</t>
   </si>
   <si>
     <r>
@@ -92,6 +87,9 @@
       <t xml:space="preserve">
 For the given friends, find the no of mutual friends</t>
     </r>
+  </si>
+  <si>
+    <t># - Mutual Friends count</t>
   </si>
 </sst>
 </file>
@@ -395,21 +393,6 @@
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,16 +417,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -471,6 +445,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,184 +806,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9B905E-6652-044B-B271-BABD64D7B8D5}">
   <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="12.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="6" width="12.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="3" width="12.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" style="1"/>
+    <col min="5" max="6" width="12.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="2:7" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="6" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="22"/>
+      <c r="E7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="20" t="s">
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="F9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="24" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="F10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="24" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
+      <c r="F12" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21" t="s">
+      <c r="C13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="22" t="s">
+      <c r="C14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="14">
+      <c r="F14" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>